<commit_message>
excluao tabelas e conserto tabela_TP
</commit_message>
<xml_diff>
--- a/Tabelas/Transformador de Potencial.xlsx
+++ b/Tabelas/Transformador de Potencial.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefetrjbr-my.sharepoint.com/personal/08951123960_cefet-rj_br/Documents/Nathan - Faculdade/8° período/EQUIPAMENTOS ELÉTRICOS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nathan Araújo\OneDrive - cefet-rj.br\Nathan - Faculdade\8° período\EQUIPAMENTOS ELÉTRICOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D0C1C6F5-523E-476A-BFE0-6D510BD1745E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{D0C1C6F5-523E-476A-BFE0-6D510BD1745E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{D3E51392-0124-4634-8071-80D177BF22B4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{E71F747A-49C7-4C8F-90A9-728871C32109}"/>
   </bookViews>
@@ -17,7 +17,8 @@
     <sheet name="6.2.2" sheetId="3" r:id="rId2"/>
     <sheet name="6.4.1" sheetId="4" r:id="rId3"/>
     <sheet name="6.4.2" sheetId="5" r:id="rId4"/>
-    <sheet name="6.6" sheetId="1" r:id="rId5"/>
+    <sheet name="6.5" sheetId="6" r:id="rId5"/>
+    <sheet name="6.6" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="40">
   <si>
     <t>6.6</t>
   </si>
@@ -151,6 +152,9 @@
   </si>
   <si>
     <t>Impedância</t>
+  </si>
+  <si>
+    <t>Regime Contínuo</t>
   </si>
 </sst>
 </file>
@@ -158,7 +162,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -193,7 +197,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1311,10 +1315,418 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3695E109-4751-4EAD-A1F2-C3F02A0AED81}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.3</v>
+      </c>
+      <c r="B1">
+        <v>0.4</v>
+      </c>
+      <c r="C1">
+        <v>0.5</v>
+      </c>
+      <c r="D1">
+        <v>0.6</v>
+      </c>
+      <c r="E1">
+        <v>0.7</v>
+      </c>
+      <c r="F1">
+        <v>0.8</v>
+      </c>
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2">
+        <v>50</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>50</v>
+      </c>
+      <c r="E2">
+        <v>40</v>
+      </c>
+      <c r="F2">
+        <v>40</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>110</v>
+      </c>
+      <c r="B3">
+        <v>90</v>
+      </c>
+      <c r="C3">
+        <v>70</v>
+      </c>
+      <c r="D3">
+        <v>70</v>
+      </c>
+      <c r="E3">
+        <v>70</v>
+      </c>
+      <c r="F3">
+        <v>60</v>
+      </c>
+      <c r="G3">
+        <v>60</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>180</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <v>120</v>
+      </c>
+      <c r="D4">
+        <v>120</v>
+      </c>
+      <c r="E4">
+        <v>110</v>
+      </c>
+      <c r="F4">
+        <v>100</v>
+      </c>
+      <c r="G4">
+        <v>80</v>
+      </c>
+      <c r="H4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>310</v>
+      </c>
+      <c r="B5">
+        <v>260</v>
+      </c>
+      <c r="C5">
+        <v>200</v>
+      </c>
+      <c r="D5">
+        <v>200</v>
+      </c>
+      <c r="E5">
+        <v>180</v>
+      </c>
+      <c r="F5">
+        <v>160</v>
+      </c>
+      <c r="G5">
+        <v>140</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>530</v>
+      </c>
+      <c r="B6">
+        <v>450</v>
+      </c>
+      <c r="C6">
+        <v>340</v>
+      </c>
+      <c r="D6">
+        <v>340</v>
+      </c>
+      <c r="E6">
+        <v>300</v>
+      </c>
+      <c r="F6">
+        <v>270</v>
+      </c>
+      <c r="G6">
+        <v>250</v>
+      </c>
+      <c r="H6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>890</v>
+      </c>
+      <c r="B7">
+        <v>750</v>
+      </c>
+      <c r="C7">
+        <v>570</v>
+      </c>
+      <c r="D7">
+        <v>570</v>
+      </c>
+      <c r="E7">
+        <v>500</v>
+      </c>
+      <c r="F7">
+        <v>500</v>
+      </c>
+      <c r="G7">
+        <v>430</v>
+      </c>
+      <c r="H7">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1470</v>
+      </c>
+      <c r="B8">
+        <v>1240</v>
+      </c>
+      <c r="C8">
+        <v>1000</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>900</v>
+      </c>
+      <c r="F8">
+        <v>850</v>
+      </c>
+      <c r="G8">
+        <v>740</v>
+      </c>
+      <c r="H8">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2480</v>
+      </c>
+      <c r="B9">
+        <v>2060</v>
+      </c>
+      <c r="C9">
+        <v>1700</v>
+      </c>
+      <c r="D9">
+        <v>1700</v>
+      </c>
+      <c r="E9">
+        <v>1500</v>
+      </c>
+      <c r="F9">
+        <v>1400</v>
+      </c>
+      <c r="G9">
+        <v>1400</v>
+      </c>
+      <c r="H9">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3300</v>
+      </c>
+      <c r="B10">
+        <v>2800</v>
+      </c>
+      <c r="C10">
+        <v>2000</v>
+      </c>
+      <c r="D10">
+        <v>2000</v>
+      </c>
+      <c r="E10">
+        <v>1900</v>
+      </c>
+      <c r="F10">
+        <v>1800</v>
+      </c>
+      <c r="G10">
+        <v>1500</v>
+      </c>
+      <c r="H10">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>5600</v>
+      </c>
+      <c r="B11">
+        <v>4700</v>
+      </c>
+      <c r="C11">
+        <v>3600</v>
+      </c>
+      <c r="D11">
+        <v>3600</v>
+      </c>
+      <c r="E11">
+        <v>3400</v>
+      </c>
+      <c r="F11">
+        <v>3000</v>
+      </c>
+      <c r="G11">
+        <v>1700</v>
+      </c>
+      <c r="H11">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>9000</v>
+      </c>
+      <c r="B12">
+        <v>7600</v>
+      </c>
+      <c r="C12">
+        <v>5900</v>
+      </c>
+      <c r="D12">
+        <v>5900</v>
+      </c>
+      <c r="E12">
+        <v>5300</v>
+      </c>
+      <c r="F12">
+        <v>5000</v>
+      </c>
+      <c r="G12">
+        <v>4500</v>
+      </c>
+      <c r="H12">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13300</v>
+      </c>
+      <c r="B13">
+        <v>11600</v>
+      </c>
+      <c r="C13">
+        <v>9400</v>
+      </c>
+      <c r="D13">
+        <v>9400</v>
+      </c>
+      <c r="E13">
+        <v>8600</v>
+      </c>
+      <c r="F13">
+        <v>8000</v>
+      </c>
+      <c r="G13">
+        <v>7900</v>
+      </c>
+      <c r="H13">
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>17500</v>
+      </c>
+      <c r="B14">
+        <v>15700</v>
+      </c>
+      <c r="C14">
+        <v>13900</v>
+      </c>
+      <c r="D14">
+        <v>13900</v>
+      </c>
+      <c r="E14">
+        <v>13000</v>
+      </c>
+      <c r="F14">
+        <v>13000</v>
+      </c>
+      <c r="G14">
+        <v>13800</v>
+      </c>
+      <c r="H14">
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>26000</v>
+      </c>
+      <c r="B15">
+        <v>24000</v>
+      </c>
+      <c r="C15">
+        <v>21300</v>
+      </c>
+      <c r="D15">
+        <v>21300</v>
+      </c>
+      <c r="E15">
+        <v>21000</v>
+      </c>
+      <c r="F15">
+        <v>20000</v>
+      </c>
+      <c r="G15">
+        <v>24000</v>
+      </c>
+      <c r="H15">
+        <v>9300</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24F82C5C-5782-4376-9191-5AC4A10C06E1}">
   <dimension ref="B1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
+    <sheetView zoomScale="165" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>